<commit_message>
updated 4.0 files and mdl
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\RMI\RMI_all_states\AL\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE1223E9-9AE7-413F-A53F-AE31470B476A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E75E9572-C6F3-4A20-81A6-2DF463EAF9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1065" windowWidth="18465" windowHeight="16935" firstSheet="1" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="2060" yWindow="2060" windowWidth="14400" windowHeight="7290" firstSheet="2" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2478,12 +2478,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2491,20 +2491,20 @@
         <v>39</v>
       </c>
       <c r="C1" s="2">
-        <v>45372</v>
+        <v>45377</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2512,17 +2512,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2563,12 +2563,12 @@
       <selection activeCell="B1" sqref="B1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2692,17 +2692,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2722,16 +2722,16 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="M7" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AE25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -4631,7 +4631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>30</v>
       </c>

</xml_diff>